<commit_message>
Updating Eggs per Bundle, Molecular, and Metadata sheet, as well as saving all files as CSV's
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Oct_2020/Wild_vs_Nurs/Molecular.sample.info.xlsx
+++ b/RAnalysis/Data/Oct_2020/Wild_vs_Nurs/Molecular.sample.info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcone\Documents\URI\Lab-Notebook\Apul_Spawning_Nurs.vs.Wild\RAnalysis\Data\Oct_2020\Wild_vs_Nurs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60A98BC-0780-4E3B-AD89-871600D705F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F992AFC-EF8C-45CC-A09E-88B44795FD40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{57A843E7-33CF-4165-992A-912C6CFCCB62}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="40">
   <si>
     <t>Date.Collected</t>
   </si>
@@ -105,6 +105,54 @@
   </si>
   <si>
     <t>Apul_241</t>
+  </si>
+  <si>
+    <t>Apul_76</t>
+  </si>
+  <si>
+    <t>Mahana</t>
+  </si>
+  <si>
+    <t>Wild</t>
+  </si>
+  <si>
+    <t>Apul_204</t>
+  </si>
+  <si>
+    <t>Apul_208</t>
+  </si>
+  <si>
+    <t>Apul_234</t>
+  </si>
+  <si>
+    <t>Apul_178</t>
+  </si>
+  <si>
+    <t>Manava</t>
+  </si>
+  <si>
+    <t>Outplant</t>
+  </si>
+  <si>
+    <t>Apul_173</t>
+  </si>
+  <si>
+    <t>Apul_66</t>
+  </si>
+  <si>
+    <t>Linareva</t>
+  </si>
+  <si>
+    <t>Apul_73</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Outplanted</t>
   </si>
 </sst>
 </file>
@@ -456,15 +504,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD777DA6-D719-42FE-AF81-41A47127F5F7}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A81"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="J127" sqref="J127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,16 +532,22 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20201007</v>
       </c>
@@ -507,13 +564,19 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20201007</v>
       </c>
@@ -530,13 +593,19 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>20201007</v>
       </c>
@@ -553,13 +622,19 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20201007</v>
       </c>
@@ -576,13 +651,19 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20201007</v>
       </c>
@@ -599,13 +680,19 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>20201007</v>
       </c>
@@ -622,13 +709,19 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20201007</v>
       </c>
@@ -645,13 +738,19 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20201007</v>
       </c>
@@ -668,13 +767,19 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>20201007</v>
       </c>
@@ -691,13 +796,19 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20201007</v>
       </c>
@@ -714,13 +825,19 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>20201007</v>
       </c>
@@ -737,13 +854,19 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>20201007</v>
       </c>
@@ -760,13 +883,19 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20201007</v>
       </c>
@@ -783,13 +912,19 @@
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20201007</v>
       </c>
@@ -806,13 +941,19 @@
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>20201007</v>
       </c>
@@ -829,13 +970,19 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20201007</v>
       </c>
@@ -852,13 +999,19 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>20201007</v>
       </c>
@@ -875,13 +1028,19 @@
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>20201007</v>
       </c>
@@ -898,13 +1057,19 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20201007</v>
       </c>
@@ -921,13 +1086,19 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20201007</v>
       </c>
@@ -944,13 +1115,19 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20201007</v>
       </c>
@@ -967,13 +1144,19 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20201007</v>
       </c>
@@ -990,13 +1173,19 @@
         <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20201007</v>
       </c>
@@ -1013,13 +1202,19 @@
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20201007</v>
       </c>
@@ -1036,13 +1231,19 @@
         <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>20201007</v>
       </c>
@@ -1059,13 +1260,19 @@
         <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>20201007</v>
       </c>
@@ -1082,13 +1289,19 @@
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>20201007</v>
       </c>
@@ -1105,13 +1318,19 @@
         <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20201007</v>
       </c>
@@ -1128,13 +1347,19 @@
         <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>20201007</v>
       </c>
@@ -1151,13 +1376,19 @@
         <v>13</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>20201007</v>
       </c>
@@ -1174,13 +1405,19 @@
         <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>20201007</v>
       </c>
@@ -1197,13 +1434,19 @@
         <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>20201007</v>
       </c>
@@ -1220,13 +1463,19 @@
         <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>20201007</v>
       </c>
@@ -1243,13 +1492,19 @@
         <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>20201007</v>
       </c>
@@ -1266,13 +1521,19 @@
         <v>22</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>20201007</v>
       </c>
@@ -1289,13 +1550,19 @@
         <v>22</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>20201007</v>
       </c>
@@ -1312,13 +1579,19 @@
         <v>23</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H37" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20201007</v>
       </c>
@@ -1335,13 +1608,19 @@
         <v>23</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H38" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20201007</v>
       </c>
@@ -1358,13 +1637,19 @@
         <v>23</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>20201007</v>
       </c>
@@ -1381,13 +1666,19 @@
         <v>23</v>
       </c>
       <c r="F40" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>20201007</v>
       </c>
@@ -1404,13 +1695,19 @@
         <v>23</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G41" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>20201007</v>
       </c>
@@ -1427,13 +1724,19 @@
         <v>9</v>
       </c>
       <c r="F42" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>20201007</v>
       </c>
@@ -1450,13 +1753,19 @@
         <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>20201007</v>
       </c>
@@ -1473,13 +1782,19 @@
         <v>9</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>20201007</v>
       </c>
@@ -1496,13 +1811,19 @@
         <v>9</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G45" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>20201007</v>
       </c>
@@ -1519,13 +1840,19 @@
         <v>9</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G46" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>20201007</v>
       </c>
@@ -1542,13 +1869,19 @@
         <v>8</v>
       </c>
       <c r="F47" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G47" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>20201007</v>
       </c>
@@ -1565,13 +1898,19 @@
         <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G48" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>20201007</v>
       </c>
@@ -1588,13 +1927,19 @@
         <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G49" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>20201007</v>
       </c>
@@ -1611,13 +1956,19 @@
         <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G50" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>20201007</v>
       </c>
@@ -1634,13 +1985,19 @@
         <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G51" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>20201007</v>
       </c>
@@ -1657,13 +2014,19 @@
         <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G52" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>20201007</v>
       </c>
@@ -1680,13 +2043,19 @@
         <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G53" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>20201007</v>
       </c>
@@ -1703,13 +2072,19 @@
         <v>10</v>
       </c>
       <c r="F54" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G54" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>20201007</v>
       </c>
@@ -1726,13 +2101,19 @@
         <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G55" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H55" t="s">
+        <v>15</v>
+      </c>
+      <c r="I55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>20201007</v>
       </c>
@@ -1749,13 +2130,19 @@
         <v>10</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G56" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>20201007</v>
       </c>
@@ -1772,13 +2159,19 @@
         <v>11</v>
       </c>
       <c r="F57" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G57" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>20201007</v>
       </c>
@@ -1795,13 +2188,19 @@
         <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G58" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>20201007</v>
       </c>
@@ -1818,13 +2217,19 @@
         <v>11</v>
       </c>
       <c r="F59" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G59" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>20201007</v>
       </c>
@@ -1841,16 +2246,22 @@
         <v>11</v>
       </c>
       <c r="F60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60" t="s">
         <v>18</v>
       </c>
-      <c r="G60" t="s">
+      <c r="I60" t="s">
         <v>18</v>
       </c>
-      <c r="H60" t="s">
+      <c r="J60" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>20201007</v>
       </c>
@@ -1867,16 +2278,22 @@
         <v>11</v>
       </c>
       <c r="F61" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" t="s">
         <v>18</v>
       </c>
-      <c r="G61" t="s">
+      <c r="I61" t="s">
         <v>18</v>
       </c>
-      <c r="H61" t="s">
+      <c r="J61" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>20201007</v>
       </c>
@@ -1893,13 +2310,19 @@
         <v>12</v>
       </c>
       <c r="F62" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G62" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H62" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>20201007</v>
       </c>
@@ -1916,13 +2339,19 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G63" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H63" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>20201007</v>
       </c>
@@ -1939,13 +2368,19 @@
         <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G64" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>20201007</v>
       </c>
@@ -1962,13 +2397,19 @@
         <v>12</v>
       </c>
       <c r="F65" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G65" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20201007</v>
       </c>
@@ -1985,13 +2426,19 @@
         <v>12</v>
       </c>
       <c r="F66" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G66" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>20201007</v>
       </c>
@@ -2008,13 +2455,19 @@
         <v>13</v>
       </c>
       <c r="F67" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G67" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H67" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20201007</v>
       </c>
@@ -2031,16 +2484,22 @@
         <v>13</v>
       </c>
       <c r="F68" t="s">
+        <v>25</v>
+      </c>
+      <c r="G68" t="s">
+        <v>26</v>
+      </c>
+      <c r="H68" t="s">
         <v>18</v>
       </c>
-      <c r="G68" t="s">
+      <c r="I68" t="s">
         <v>18</v>
       </c>
-      <c r="H68" t="s">
+      <c r="J68" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20201007</v>
       </c>
@@ -2057,16 +2516,22 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
+        <v>25</v>
+      </c>
+      <c r="G69" t="s">
+        <v>26</v>
+      </c>
+      <c r="H69" t="s">
         <v>18</v>
       </c>
-      <c r="G69" t="s">
+      <c r="I69" t="s">
         <v>18</v>
       </c>
-      <c r="H69" t="s">
+      <c r="J69" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>20201007</v>
       </c>
@@ -2083,16 +2548,22 @@
         <v>13</v>
       </c>
       <c r="F70" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" t="s">
+        <v>26</v>
+      </c>
+      <c r="H70" t="s">
         <v>18</v>
       </c>
-      <c r="G70" t="s">
+      <c r="I70" t="s">
         <v>18</v>
       </c>
-      <c r="H70" t="s">
+      <c r="J70" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>20201007</v>
       </c>
@@ -2109,16 +2580,22 @@
         <v>13</v>
       </c>
       <c r="F71" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" t="s">
         <v>18</v>
       </c>
-      <c r="G71" t="s">
+      <c r="I71" t="s">
         <v>18</v>
       </c>
-      <c r="H71" t="s">
+      <c r="J71" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>20201007</v>
       </c>
@@ -2135,16 +2612,22 @@
         <v>22</v>
       </c>
       <c r="F72" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" t="s">
+        <v>26</v>
+      </c>
+      <c r="H72" t="s">
         <v>18</v>
       </c>
-      <c r="G72" t="s">
+      <c r="I72" t="s">
         <v>18</v>
       </c>
-      <c r="H72" t="s">
+      <c r="J72" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>20201007</v>
       </c>
@@ -2161,16 +2644,22 @@
         <v>22</v>
       </c>
       <c r="F73" t="s">
+        <v>25</v>
+      </c>
+      <c r="G73" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" t="s">
         <v>18</v>
       </c>
-      <c r="G73" t="s">
+      <c r="I73" t="s">
         <v>18</v>
       </c>
-      <c r="H73" t="s">
+      <c r="J73" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>20201007</v>
       </c>
@@ -2187,16 +2676,22 @@
         <v>22</v>
       </c>
       <c r="F74" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" t="s">
+        <v>26</v>
+      </c>
+      <c r="H74" t="s">
         <v>18</v>
       </c>
-      <c r="G74" t="s">
+      <c r="I74" t="s">
         <v>18</v>
       </c>
-      <c r="H74" t="s">
+      <c r="J74" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>20201007</v>
       </c>
@@ -2213,16 +2708,22 @@
         <v>22</v>
       </c>
       <c r="F75" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H75" t="s">
         <v>18</v>
       </c>
-      <c r="G75" t="s">
+      <c r="I75" t="s">
         <v>18</v>
       </c>
-      <c r="H75" t="s">
+      <c r="J75" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>20201007</v>
       </c>
@@ -2239,16 +2740,22 @@
         <v>22</v>
       </c>
       <c r="F76" t="s">
+        <v>25</v>
+      </c>
+      <c r="G76" t="s">
+        <v>26</v>
+      </c>
+      <c r="H76" t="s">
         <v>18</v>
       </c>
-      <c r="G76" t="s">
+      <c r="I76" t="s">
         <v>18</v>
       </c>
-      <c r="H76" t="s">
+      <c r="J76" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>20201007</v>
       </c>
@@ -2265,16 +2772,22 @@
         <v>23</v>
       </c>
       <c r="F77" t="s">
+        <v>25</v>
+      </c>
+      <c r="G77" t="s">
+        <v>39</v>
+      </c>
+      <c r="H77" t="s">
         <v>18</v>
       </c>
-      <c r="G77" t="s">
+      <c r="I77" t="s">
         <v>18</v>
       </c>
-      <c r="H77" t="s">
+      <c r="J77" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>20201007</v>
       </c>
@@ -2291,16 +2804,22 @@
         <v>23</v>
       </c>
       <c r="F78" t="s">
+        <v>25</v>
+      </c>
+      <c r="G78" t="s">
+        <v>39</v>
+      </c>
+      <c r="H78" t="s">
         <v>18</v>
       </c>
-      <c r="G78" t="s">
+      <c r="I78" t="s">
         <v>18</v>
       </c>
-      <c r="H78" t="s">
+      <c r="J78" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>20201007</v>
       </c>
@@ -2317,16 +2836,22 @@
         <v>23</v>
       </c>
       <c r="F79" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" t="s">
+        <v>39</v>
+      </c>
+      <c r="H79" t="s">
         <v>18</v>
       </c>
-      <c r="G79" t="s">
+      <c r="I79" t="s">
         <v>18</v>
       </c>
-      <c r="H79" t="s">
+      <c r="J79" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>20201007</v>
       </c>
@@ -2343,16 +2868,22 @@
         <v>23</v>
       </c>
       <c r="F80" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" t="s">
+        <v>39</v>
+      </c>
+      <c r="H80" t="s">
         <v>18</v>
       </c>
-      <c r="G80" t="s">
+      <c r="I80" t="s">
         <v>18</v>
       </c>
-      <c r="H80" t="s">
+      <c r="J80" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20201007</v>
       </c>
@@ -2369,13 +2900,1585 @@
         <v>23</v>
       </c>
       <c r="F81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" t="s">
+        <v>39</v>
+      </c>
+      <c r="H81" t="s">
         <v>18</v>
       </c>
-      <c r="G81" t="s">
+      <c r="I81" t="s">
         <v>18</v>
       </c>
-      <c r="H81" t="s">
+      <c r="J81" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>20201009</v>
+      </c>
+      <c r="B82">
+        <v>253</v>
+      </c>
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82">
+        <v>76</v>
+      </c>
+      <c r="E82" t="s">
+        <v>24</v>
+      </c>
+      <c r="F82" t="s">
+        <v>25</v>
+      </c>
+      <c r="G82" t="s">
+        <v>26</v>
+      </c>
+      <c r="H82" t="s">
+        <v>14</v>
+      </c>
+      <c r="I82" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>20201009</v>
+      </c>
+      <c r="B83">
+        <v>254</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83">
+        <v>76</v>
+      </c>
+      <c r="E83" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" t="s">
+        <v>26</v>
+      </c>
+      <c r="H83" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>20201009</v>
+      </c>
+      <c r="B84">
+        <v>255</v>
+      </c>
+      <c r="C84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84">
+        <v>76</v>
+      </c>
+      <c r="E84" t="s">
+        <v>24</v>
+      </c>
+      <c r="F84" t="s">
+        <v>25</v>
+      </c>
+      <c r="G84" t="s">
+        <v>26</v>
+      </c>
+      <c r="H84" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>20201009</v>
+      </c>
+      <c r="B85">
+        <v>256</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85">
+        <v>204</v>
+      </c>
+      <c r="E85" t="s">
+        <v>27</v>
+      </c>
+      <c r="F85" t="s">
+        <v>25</v>
+      </c>
+      <c r="G85" t="s">
+        <v>26</v>
+      </c>
+      <c r="H85" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>20201009</v>
+      </c>
+      <c r="B86">
+        <v>257</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86">
+        <v>204</v>
+      </c>
+      <c r="E86" t="s">
+        <v>27</v>
+      </c>
+      <c r="F86" t="s">
+        <v>25</v>
+      </c>
+      <c r="G86" t="s">
+        <v>26</v>
+      </c>
+      <c r="H86" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>20201009</v>
+      </c>
+      <c r="B87">
+        <v>258</v>
+      </c>
+      <c r="C87" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87">
+        <v>204</v>
+      </c>
+      <c r="E87" t="s">
+        <v>27</v>
+      </c>
+      <c r="F87" t="s">
+        <v>25</v>
+      </c>
+      <c r="G87" t="s">
+        <v>26</v>
+      </c>
+      <c r="H87" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>20201009</v>
+      </c>
+      <c r="B88">
+        <v>259</v>
+      </c>
+      <c r="C88" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88">
+        <v>208</v>
+      </c>
+      <c r="E88" t="s">
+        <v>28</v>
+      </c>
+      <c r="F88" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" t="s">
+        <v>26</v>
+      </c>
+      <c r="H88" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>20201009</v>
+      </c>
+      <c r="B89">
+        <v>260</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89">
+        <v>208</v>
+      </c>
+      <c r="E89" t="s">
+        <v>28</v>
+      </c>
+      <c r="F89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" t="s">
+        <v>26</v>
+      </c>
+      <c r="H89" t="s">
+        <v>14</v>
+      </c>
+      <c r="I89" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>20201009</v>
+      </c>
+      <c r="B90">
+        <v>261</v>
+      </c>
+      <c r="C90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90">
+        <v>208</v>
+      </c>
+      <c r="E90" t="s">
+        <v>28</v>
+      </c>
+      <c r="F90" t="s">
+        <v>25</v>
+      </c>
+      <c r="G90" t="s">
+        <v>26</v>
+      </c>
+      <c r="H90" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>20201009</v>
+      </c>
+      <c r="B91">
+        <v>262</v>
+      </c>
+      <c r="C91" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91">
+        <v>234</v>
+      </c>
+      <c r="E91" t="s">
+        <v>29</v>
+      </c>
+      <c r="F91" t="s">
+        <v>25</v>
+      </c>
+      <c r="G91" t="s">
+        <v>26</v>
+      </c>
+      <c r="H91" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>20201009</v>
+      </c>
+      <c r="B92">
+        <v>263</v>
+      </c>
+      <c r="C92" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92">
+        <v>234</v>
+      </c>
+      <c r="E92" t="s">
+        <v>29</v>
+      </c>
+      <c r="F92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" t="s">
+        <v>26</v>
+      </c>
+      <c r="H92" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>20201009</v>
+      </c>
+      <c r="B93">
+        <v>264</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93">
+        <v>234</v>
+      </c>
+      <c r="E93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93" t="s">
+        <v>25</v>
+      </c>
+      <c r="G93" t="s">
+        <v>26</v>
+      </c>
+      <c r="H93" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>20201009</v>
+      </c>
+      <c r="B94">
+        <v>265</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94">
+        <v>178</v>
+      </c>
+      <c r="E94" t="s">
+        <v>30</v>
+      </c>
+      <c r="F94" t="s">
+        <v>31</v>
+      </c>
+      <c r="G94" t="s">
+        <v>32</v>
+      </c>
+      <c r="H94" t="s">
+        <v>14</v>
+      </c>
+      <c r="I94" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>20201009</v>
+      </c>
+      <c r="B95">
+        <v>266</v>
+      </c>
+      <c r="C95" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95">
+        <v>178</v>
+      </c>
+      <c r="E95" t="s">
+        <v>30</v>
+      </c>
+      <c r="F95" t="s">
+        <v>31</v>
+      </c>
+      <c r="G95" t="s">
+        <v>32</v>
+      </c>
+      <c r="H95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I95" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>20201009</v>
+      </c>
+      <c r="B96">
+        <v>267</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96">
+        <v>178</v>
+      </c>
+      <c r="E96" t="s">
+        <v>30</v>
+      </c>
+      <c r="F96" t="s">
+        <v>31</v>
+      </c>
+      <c r="G96" t="s">
+        <v>32</v>
+      </c>
+      <c r="H96" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>20201009</v>
+      </c>
+      <c r="B97">
+        <v>268</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97">
+        <v>173</v>
+      </c>
+      <c r="E97" t="s">
+        <v>33</v>
+      </c>
+      <c r="F97" t="s">
+        <v>31</v>
+      </c>
+      <c r="G97" t="s">
+        <v>32</v>
+      </c>
+      <c r="H97" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>20201009</v>
+      </c>
+      <c r="B98">
+        <v>269</v>
+      </c>
+      <c r="C98" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98">
+        <v>173</v>
+      </c>
+      <c r="E98" t="s">
+        <v>33</v>
+      </c>
+      <c r="F98" t="s">
+        <v>31</v>
+      </c>
+      <c r="G98" t="s">
+        <v>32</v>
+      </c>
+      <c r="H98" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>20201009</v>
+      </c>
+      <c r="B99">
+        <v>270</v>
+      </c>
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99">
+        <v>173</v>
+      </c>
+      <c r="E99" t="s">
+        <v>33</v>
+      </c>
+      <c r="F99" t="s">
+        <v>31</v>
+      </c>
+      <c r="G99" t="s">
+        <v>32</v>
+      </c>
+      <c r="H99" t="s">
+        <v>14</v>
+      </c>
+      <c r="I99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>20201009</v>
+      </c>
+      <c r="B100">
+        <v>271</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100">
+        <v>66</v>
+      </c>
+      <c r="E100" t="s">
+        <v>34</v>
+      </c>
+      <c r="F100" t="s">
+        <v>35</v>
+      </c>
+      <c r="G100" t="s">
+        <v>26</v>
+      </c>
+      <c r="H100" t="s">
+        <v>15</v>
+      </c>
+      <c r="I100" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>20201009</v>
+      </c>
+      <c r="B101">
+        <v>272</v>
+      </c>
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101">
+        <v>66</v>
+      </c>
+      <c r="E101" t="s">
+        <v>34</v>
+      </c>
+      <c r="F101" t="s">
+        <v>35</v>
+      </c>
+      <c r="G101" t="s">
+        <v>26</v>
+      </c>
+      <c r="H101" t="s">
+        <v>15</v>
+      </c>
+      <c r="I101" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>20201009</v>
+      </c>
+      <c r="B102">
+        <v>273</v>
+      </c>
+      <c r="C102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102">
+        <v>66</v>
+      </c>
+      <c r="E102" t="s">
+        <v>34</v>
+      </c>
+      <c r="F102" t="s">
+        <v>35</v>
+      </c>
+      <c r="G102" t="s">
+        <v>26</v>
+      </c>
+      <c r="H102" t="s">
+        <v>15</v>
+      </c>
+      <c r="I102" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>20201009</v>
+      </c>
+      <c r="B103">
+        <v>274</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103">
+        <v>173</v>
+      </c>
+      <c r="E103" t="s">
+        <v>33</v>
+      </c>
+      <c r="F103" t="s">
+        <v>31</v>
+      </c>
+      <c r="G103" t="s">
+        <v>32</v>
+      </c>
+      <c r="H103" t="s">
+        <v>15</v>
+      </c>
+      <c r="I103" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>20201009</v>
+      </c>
+      <c r="B104">
+        <v>275</v>
+      </c>
+      <c r="C104" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104">
+        <v>173</v>
+      </c>
+      <c r="E104" t="s">
+        <v>33</v>
+      </c>
+      <c r="F104" t="s">
+        <v>31</v>
+      </c>
+      <c r="G104" t="s">
+        <v>32</v>
+      </c>
+      <c r="H104" t="s">
+        <v>15</v>
+      </c>
+      <c r="I104" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>20201009</v>
+      </c>
+      <c r="B105">
+        <v>276</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105">
+        <v>173</v>
+      </c>
+      <c r="E105" t="s">
+        <v>33</v>
+      </c>
+      <c r="F105" t="s">
+        <v>31</v>
+      </c>
+      <c r="G105" t="s">
+        <v>32</v>
+      </c>
+      <c r="H105" t="s">
+        <v>15</v>
+      </c>
+      <c r="I105" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>20201009</v>
+      </c>
+      <c r="B106">
+        <v>277</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106">
+        <v>178</v>
+      </c>
+      <c r="E106" t="s">
+        <v>30</v>
+      </c>
+      <c r="F106" t="s">
+        <v>31</v>
+      </c>
+      <c r="G106" t="s">
+        <v>32</v>
+      </c>
+      <c r="H106" t="s">
+        <v>15</v>
+      </c>
+      <c r="I106" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>20201009</v>
+      </c>
+      <c r="B107">
+        <v>278</v>
+      </c>
+      <c r="C107" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107">
+        <v>178</v>
+      </c>
+      <c r="E107" t="s">
+        <v>30</v>
+      </c>
+      <c r="F107" t="s">
+        <v>31</v>
+      </c>
+      <c r="G107" t="s">
+        <v>32</v>
+      </c>
+      <c r="H107" t="s">
+        <v>15</v>
+      </c>
+      <c r="I107" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>20201009</v>
+      </c>
+      <c r="B108">
+        <v>279</v>
+      </c>
+      <c r="C108" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108">
+        <v>178</v>
+      </c>
+      <c r="E108" t="s">
+        <v>30</v>
+      </c>
+      <c r="F108" t="s">
+        <v>31</v>
+      </c>
+      <c r="G108" t="s">
+        <v>32</v>
+      </c>
+      <c r="H108" t="s">
+        <v>15</v>
+      </c>
+      <c r="I108" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>20201009</v>
+      </c>
+      <c r="B109">
+        <v>280</v>
+      </c>
+      <c r="C109" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109">
+        <v>73</v>
+      </c>
+      <c r="E109" t="s">
+        <v>36</v>
+      </c>
+      <c r="F109" t="s">
+        <v>35</v>
+      </c>
+      <c r="G109" t="s">
+        <v>26</v>
+      </c>
+      <c r="H109" t="s">
+        <v>15</v>
+      </c>
+      <c r="I109" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>20201009</v>
+      </c>
+      <c r="B110">
+        <v>281</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110">
+        <v>73</v>
+      </c>
+      <c r="E110" t="s">
+        <v>36</v>
+      </c>
+      <c r="F110" t="s">
+        <v>35</v>
+      </c>
+      <c r="G110" t="s">
+        <v>26</v>
+      </c>
+      <c r="H110" t="s">
+        <v>15</v>
+      </c>
+      <c r="I110" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>20201009</v>
+      </c>
+      <c r="B111">
+        <v>282</v>
+      </c>
+      <c r="C111" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111">
+        <v>73</v>
+      </c>
+      <c r="E111" t="s">
+        <v>36</v>
+      </c>
+      <c r="F111" t="s">
+        <v>35</v>
+      </c>
+      <c r="G111" t="s">
+        <v>26</v>
+      </c>
+      <c r="H111" t="s">
+        <v>15</v>
+      </c>
+      <c r="I111" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>20201009</v>
+      </c>
+      <c r="B112">
+        <v>283</v>
+      </c>
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112">
+        <v>241</v>
+      </c>
+      <c r="E112" t="s">
+        <v>23</v>
+      </c>
+      <c r="F112" t="s">
+        <v>25</v>
+      </c>
+      <c r="G112" t="s">
+        <v>32</v>
+      </c>
+      <c r="H112" t="s">
+        <v>15</v>
+      </c>
+      <c r="I112" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>20201009</v>
+      </c>
+      <c r="B113">
+        <v>284</v>
+      </c>
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113">
+        <v>241</v>
+      </c>
+      <c r="E113" t="s">
+        <v>23</v>
+      </c>
+      <c r="F113" t="s">
+        <v>25</v>
+      </c>
+      <c r="G113" t="s">
+        <v>32</v>
+      </c>
+      <c r="H113" t="s">
+        <v>15</v>
+      </c>
+      <c r="I113" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>20201009</v>
+      </c>
+      <c r="B114">
+        <v>285</v>
+      </c>
+      <c r="C114" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114">
+        <v>241</v>
+      </c>
+      <c r="E114" t="s">
+        <v>23</v>
+      </c>
+      <c r="F114" t="s">
+        <v>25</v>
+      </c>
+      <c r="G114" t="s">
+        <v>32</v>
+      </c>
+      <c r="H114" t="s">
+        <v>15</v>
+      </c>
+      <c r="I114" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>20201009</v>
+      </c>
+      <c r="B115">
+        <v>286</v>
+      </c>
+      <c r="C115" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115">
+        <v>208</v>
+      </c>
+      <c r="E115" t="s">
+        <v>28</v>
+      </c>
+      <c r="F115" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" t="s">
+        <v>26</v>
+      </c>
+      <c r="H115" t="s">
+        <v>15</v>
+      </c>
+      <c r="I115" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>20201009</v>
+      </c>
+      <c r="B116">
+        <v>287</v>
+      </c>
+      <c r="C116" t="s">
+        <v>7</v>
+      </c>
+      <c r="D116">
+        <v>208</v>
+      </c>
+      <c r="E116" t="s">
+        <v>28</v>
+      </c>
+      <c r="F116" t="s">
+        <v>25</v>
+      </c>
+      <c r="G116" t="s">
+        <v>26</v>
+      </c>
+      <c r="H116" t="s">
+        <v>15</v>
+      </c>
+      <c r="I116" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>20201009</v>
+      </c>
+      <c r="B117">
+        <v>288</v>
+      </c>
+      <c r="C117" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117">
+        <v>208</v>
+      </c>
+      <c r="E117" t="s">
+        <v>28</v>
+      </c>
+      <c r="F117" t="s">
+        <v>25</v>
+      </c>
+      <c r="G117" t="s">
+        <v>26</v>
+      </c>
+      <c r="H117" t="s">
+        <v>15</v>
+      </c>
+      <c r="I117" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>20201009</v>
+      </c>
+      <c r="B118">
+        <v>289</v>
+      </c>
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118">
+        <v>234</v>
+      </c>
+      <c r="E118" t="s">
+        <v>29</v>
+      </c>
+      <c r="F118" t="s">
+        <v>25</v>
+      </c>
+      <c r="G118" t="s">
+        <v>32</v>
+      </c>
+      <c r="H118" t="s">
+        <v>15</v>
+      </c>
+      <c r="I118" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>20201009</v>
+      </c>
+      <c r="B119">
+        <v>290</v>
+      </c>
+      <c r="C119" t="s">
+        <v>7</v>
+      </c>
+      <c r="D119">
+        <v>234</v>
+      </c>
+      <c r="E119" t="s">
+        <v>29</v>
+      </c>
+      <c r="F119" t="s">
+        <v>25</v>
+      </c>
+      <c r="G119" t="s">
+        <v>32</v>
+      </c>
+      <c r="H119" t="s">
+        <v>15</v>
+      </c>
+      <c r="I119" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>20201009</v>
+      </c>
+      <c r="B120">
+        <v>291</v>
+      </c>
+      <c r="C120" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120">
+        <v>234</v>
+      </c>
+      <c r="E120" t="s">
+        <v>29</v>
+      </c>
+      <c r="F120" t="s">
+        <v>25</v>
+      </c>
+      <c r="G120" t="s">
+        <v>32</v>
+      </c>
+      <c r="H120" t="s">
+        <v>15</v>
+      </c>
+      <c r="I120" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>20201009</v>
+      </c>
+      <c r="B121">
+        <v>292</v>
+      </c>
+      <c r="C121" t="s">
+        <v>7</v>
+      </c>
+      <c r="D121">
+        <v>76</v>
+      </c>
+      <c r="E121" t="s">
+        <v>24</v>
+      </c>
+      <c r="F121" t="s">
+        <v>25</v>
+      </c>
+      <c r="G121" t="s">
+        <v>26</v>
+      </c>
+      <c r="H121" t="s">
+        <v>15</v>
+      </c>
+      <c r="I121" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>20201009</v>
+      </c>
+      <c r="B122">
+        <v>293</v>
+      </c>
+      <c r="C122" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122">
+        <v>76</v>
+      </c>
+      <c r="E122" t="s">
+        <v>24</v>
+      </c>
+      <c r="F122" t="s">
+        <v>25</v>
+      </c>
+      <c r="G122" t="s">
+        <v>26</v>
+      </c>
+      <c r="H122" t="s">
+        <v>15</v>
+      </c>
+      <c r="I122" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>20201009</v>
+      </c>
+      <c r="B123">
+        <v>294</v>
+      </c>
+      <c r="C123" t="s">
+        <v>7</v>
+      </c>
+      <c r="D123">
+        <v>76</v>
+      </c>
+      <c r="E123" t="s">
+        <v>24</v>
+      </c>
+      <c r="F123" t="s">
+        <v>25</v>
+      </c>
+      <c r="G123" t="s">
+        <v>26</v>
+      </c>
+      <c r="H123" t="s">
+        <v>15</v>
+      </c>
+      <c r="I123" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>20201009</v>
+      </c>
+      <c r="B124">
+        <v>295</v>
+      </c>
+      <c r="C124" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124">
+        <v>204</v>
+      </c>
+      <c r="E124" t="s">
+        <v>27</v>
+      </c>
+      <c r="F124" t="s">
+        <v>25</v>
+      </c>
+      <c r="G124" t="s">
+        <v>26</v>
+      </c>
+      <c r="H124" t="s">
+        <v>15</v>
+      </c>
+      <c r="I124" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>20201009</v>
+      </c>
+      <c r="B125">
+        <v>296</v>
+      </c>
+      <c r="C125" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125">
+        <v>204</v>
+      </c>
+      <c r="E125" t="s">
+        <v>27</v>
+      </c>
+      <c r="F125" t="s">
+        <v>25</v>
+      </c>
+      <c r="G125" t="s">
+        <v>26</v>
+      </c>
+      <c r="H125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I125" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>20201009</v>
+      </c>
+      <c r="B126">
+        <v>297</v>
+      </c>
+      <c r="C126" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126">
+        <v>204</v>
+      </c>
+      <c r="E126" t="s">
+        <v>27</v>
+      </c>
+      <c r="F126" t="s">
+        <v>25</v>
+      </c>
+      <c r="G126" t="s">
+        <v>26</v>
+      </c>
+      <c r="H126" t="s">
+        <v>15</v>
+      </c>
+      <c r="I126" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>20201009</v>
+      </c>
+      <c r="B127">
+        <v>325</v>
+      </c>
+      <c r="C127" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127">
+        <v>241</v>
+      </c>
+      <c r="E127" t="s">
+        <v>23</v>
+      </c>
+      <c r="F127" t="s">
+        <v>25</v>
+      </c>
+      <c r="G127" t="s">
+        <v>32</v>
+      </c>
+      <c r="H127" t="s">
+        <v>14</v>
+      </c>
+      <c r="I127" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>20201009</v>
+      </c>
+      <c r="B128">
+        <v>326</v>
+      </c>
+      <c r="C128" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128">
+        <v>241</v>
+      </c>
+      <c r="E128" t="s">
+        <v>23</v>
+      </c>
+      <c r="F128" t="s">
+        <v>25</v>
+      </c>
+      <c r="G128" t="s">
+        <v>32</v>
+      </c>
+      <c r="H128" t="s">
+        <v>14</v>
+      </c>
+      <c r="I128" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>20201009</v>
+      </c>
+      <c r="B129">
+        <v>327</v>
+      </c>
+      <c r="C129" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129">
+        <v>241</v>
+      </c>
+      <c r="E129" t="s">
+        <v>23</v>
+      </c>
+      <c r="F129" t="s">
+        <v>25</v>
+      </c>
+      <c r="G129" t="s">
+        <v>32</v>
+      </c>
+      <c r="H129" t="s">
+        <v>14</v>
+      </c>
+      <c r="I129" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>20201009</v>
+      </c>
+      <c r="B130">
+        <v>328</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130">
+        <v>66</v>
+      </c>
+      <c r="E130" t="s">
+        <v>34</v>
+      </c>
+      <c r="F130" t="s">
+        <v>35</v>
+      </c>
+      <c r="G130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H130" t="s">
+        <v>14</v>
+      </c>
+      <c r="I130" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>20201009</v>
+      </c>
+      <c r="B131">
+        <v>329</v>
+      </c>
+      <c r="C131" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131">
+        <v>66</v>
+      </c>
+      <c r="E131" t="s">
+        <v>34</v>
+      </c>
+      <c r="F131" t="s">
+        <v>35</v>
+      </c>
+      <c r="G131" t="s">
+        <v>26</v>
+      </c>
+      <c r="H131" t="s">
+        <v>14</v>
+      </c>
+      <c r="I131" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>20201009</v>
+      </c>
+      <c r="B132">
+        <v>330</v>
+      </c>
+      <c r="C132" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132">
+        <v>66</v>
+      </c>
+      <c r="E132" t="s">
+        <v>34</v>
+      </c>
+      <c r="F132" t="s">
+        <v>35</v>
+      </c>
+      <c r="G132" t="s">
+        <v>26</v>
+      </c>
+      <c r="H132" t="s">
+        <v>14</v>
+      </c>
+      <c r="I132" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>20201009</v>
+      </c>
+      <c r="B133">
+        <v>331</v>
+      </c>
+      <c r="C133" t="s">
+        <v>7</v>
+      </c>
+      <c r="D133">
+        <v>73</v>
+      </c>
+      <c r="E133" t="s">
+        <v>36</v>
+      </c>
+      <c r="F133" t="s">
+        <v>35</v>
+      </c>
+      <c r="G133" t="s">
+        <v>26</v>
+      </c>
+      <c r="H133" t="s">
+        <v>14</v>
+      </c>
+      <c r="I133" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>20201009</v>
+      </c>
+      <c r="B134">
+        <v>332</v>
+      </c>
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134">
+        <v>73</v>
+      </c>
+      <c r="E134" t="s">
+        <v>36</v>
+      </c>
+      <c r="F134" t="s">
+        <v>35</v>
+      </c>
+      <c r="G134" t="s">
+        <v>26</v>
+      </c>
+      <c r="H134" t="s">
+        <v>14</v>
+      </c>
+      <c r="I134" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>20201009</v>
+      </c>
+      <c r="B135">
+        <v>333</v>
+      </c>
+      <c r="C135" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135">
+        <v>73</v>
+      </c>
+      <c r="E135" t="s">
+        <v>36</v>
+      </c>
+      <c r="F135" t="s">
+        <v>35</v>
+      </c>
+      <c r="G135" t="s">
+        <v>26</v>
+      </c>
+      <c r="H135" t="s">
+        <v>14</v>
+      </c>
+      <c r="I135" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>